<commit_message>
Update artist field to be important
</commit_message>
<xml_diff>
--- a/Data Dict/Data_Dict_V0.07.xlsx
+++ b/Data Dict/Data_Dict_V0.07.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/both/Desktop/MDS/Semester_3/Data Sci project/Data Dict/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/both/Github_path/Data-Science-Project_Gr7/Data Dict/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED59BEDA-7361-A646-A310-BB1910C8BFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730F4118-0A68-7741-BC01-1E574217C6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="395">
   <si>
     <t>Version</t>
   </si>
@@ -1229,6 +1229,9 @@
   </si>
   <si>
     <t>If value is blank? Remove ? Ex p0820 Do we still need this field</t>
+  </si>
+  <si>
+    <t>To find the relationship between material and artist</t>
   </si>
 </sst>
 </file>
@@ -1657,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -1773,10 +1776,18 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="26">
+        <v>44692</v>
+      </c>
     </row>
     <row r="12" spans="2:5" ht="15.75" customHeight="1">
       <c r="B12" s="2"/>
@@ -7669,8 +7680,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B184" sqref="B184"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C214" sqref="C214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -7678,10 +7689,10 @@
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="47.33203125" customWidth="1"/>
     <col min="3" max="3" width="30.1640625" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" customWidth="1"/>
     <col min="8" max="8" width="121" bestFit="1" customWidth="1"/>
     <col min="9" max="26" width="10.5" customWidth="1"/>
   </cols>
@@ -7781,9 +7792,11 @@
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="17" t="s">
-        <v>335</v>
-      </c>
-      <c r="H5" s="17"/>
+        <v>48</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A6" s="16">

</xml_diff>